<commit_message>
Added several different templates, standup guidelines, frameworks about our group
</commit_message>
<xml_diff>
--- a/Done/Sprint_Burndown_Chart_Template.xlsx
+++ b/Done/Sprint_Burndown_Chart_Template.xlsx
@@ -226,7 +226,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Day 1</t>
   </si>
@@ -286,9 +286,6 @@
     <t>Day 10</t>
   </si>
   <si>
-    <t>Example Product Backlog Item (PBI)  Estimated During Sprint Planning</t>
-  </si>
-  <si>
     <t>Backlog Item ID</t>
   </si>
   <si>
@@ -311,6 +308,12 @@
   </si>
   <si>
     <t>Example unstarted task that isn't in current sprint 2</t>
+  </si>
+  <si>
+    <t>Create Account</t>
+  </si>
+  <si>
+    <t>Adasd</t>
   </si>
 </sst>
 </file>
@@ -904,7 +907,7 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -985,7 +988,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
@@ -1025,12 +1027,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="16" fontId="3" fillId="10" borderId="21" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1044,6 +1040,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="14" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1183,37 +1185,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1258,37 +1260,37 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.3</c:v>
+                  <c:v>15.3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.6</c:v>
+                  <c:v>13.600000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.8999999999999995</c:v>
+                  <c:v>11.900000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.1999999999999993</c:v>
+                  <c:v>10.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.4999999999999991</c:v>
+                  <c:v>8.5000000000000036</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.7999999999999989</c:v>
+                  <c:v>6.8000000000000034</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.0999999999999988</c:v>
+                  <c:v>5.1000000000000032</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.3999999999999988</c:v>
+                  <c:v>3.400000000000003</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.69999999999999885</c:v>
+                  <c:v>1.7000000000000031</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-1.1102230246251565E-15</c:v>
+                  <c:v>3.1086244689504383E-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1772,8 +1774,8 @@
   </sheetPr>
   <dimension ref="A1:X42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1788,57 +1790,57 @@
   <sheetData>
     <row r="1" spans="1:23" ht="49.8" x14ac:dyDescent="0.8">
       <c r="A1" s="36"/>
-      <c r="B1" s="72" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72"/>
-      <c r="J1" s="72"/>
-      <c r="K1" s="72"/>
-      <c r="L1" s="72"/>
-      <c r="M1" s="72"/>
-      <c r="N1" s="72"/>
-      <c r="O1" s="72"/>
-      <c r="P1" s="72"/>
-      <c r="Q1" s="72"/>
-      <c r="R1" s="72"/>
-      <c r="S1" s="72"/>
-      <c r="T1" s="72"/>
-      <c r="U1" s="72"/>
-      <c r="V1" s="72"/>
-      <c r="W1" s="72"/>
+      <c r="B1" s="76" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="76"/>
+      <c r="O1" s="76"/>
+      <c r="P1" s="76"/>
+      <c r="Q1" s="76"/>
+      <c r="R1" s="76"/>
+      <c r="S1" s="76"/>
+      <c r="T1" s="76"/>
+      <c r="U1" s="76"/>
+      <c r="V1" s="76"/>
+      <c r="W1" s="76"/>
     </row>
     <row r="2" spans="1:23" ht="33" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" s="36"/>
-      <c r="B2" s="73" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="73"/>
-      <c r="M2" s="73"/>
-      <c r="N2" s="73"/>
-      <c r="O2" s="73"/>
-      <c r="P2" s="73"/>
-      <c r="Q2" s="73"/>
-      <c r="R2" s="73"/>
-      <c r="S2" s="73"/>
-      <c r="T2" s="73"/>
-      <c r="U2" s="73"/>
-      <c r="V2" s="73"/>
-      <c r="W2" s="73"/>
+      <c r="B2" s="77" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="77"/>
+      <c r="L2" s="77"/>
+      <c r="M2" s="77"/>
+      <c r="N2" s="77"/>
+      <c r="O2" s="77"/>
+      <c r="P2" s="77"/>
+      <c r="Q2" s="77"/>
+      <c r="R2" s="77"/>
+      <c r="S2" s="77"/>
+      <c r="T2" s="77"/>
+      <c r="U2" s="77"/>
+      <c r="V2" s="77"/>
+      <c r="W2" s="77"/>
     </row>
     <row r="3" spans="1:23" s="2" customFormat="1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="34"/>
@@ -1862,50 +1864,50 @@
       <c r="S3" s="43"/>
       <c r="T3" s="43"/>
       <c r="U3" s="43"/>
-      <c r="V3" s="71"/>
+      <c r="V3" s="70"/>
       <c r="W3" s="44"/>
     </row>
     <row r="4" spans="1:23" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="35"/>
       <c r="B4" s="37"/>
       <c r="C4" s="45" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" s="46" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="47"/>
-      <c r="F4" s="56">
+      <c r="F4" s="55">
         <v>42814</v>
       </c>
-      <c r="G4" s="57">
+      <c r="G4" s="56">
         <v>42815</v>
       </c>
-      <c r="H4" s="56">
+      <c r="H4" s="55">
         <v>42816</v>
       </c>
-      <c r="I4" s="74">
+      <c r="I4" s="71">
         <v>42817</v>
       </c>
-      <c r="J4" s="56">
+      <c r="J4" s="55">
         <v>42818</v>
       </c>
-      <c r="K4" s="57">
+      <c r="K4" s="56">
         <v>42821</v>
       </c>
-      <c r="L4" s="56">
+      <c r="L4" s="55">
         <v>42822</v>
       </c>
-      <c r="M4" s="57">
+      <c r="M4" s="56">
         <v>42823</v>
       </c>
-      <c r="N4" s="76">
+      <c r="N4" s="73">
         <v>42824</v>
       </c>
-      <c r="O4" s="57">
+      <c r="O4" s="56">
         <v>42825</v>
       </c>
-      <c r="P4" s="77"/>
+      <c r="P4" s="74"/>
       <c r="Q4" s="38"/>
       <c r="R4" s="38"/>
       <c r="S4" s="38"/>
@@ -1930,7 +1932,7 @@
       <c r="H5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="75" t="s">
+      <c r="I5" s="72" t="s">
         <v>3</v>
       </c>
       <c r="J5" s="12" t="s">
@@ -1945,14 +1947,14 @@
       <c r="M5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="N5" s="75" t="s">
+      <c r="N5" s="72" t="s">
         <v>8</v>
       </c>
       <c r="O5" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="P5" s="78" t="s">
-        <v>24</v>
+      <c r="P5" s="75" t="s">
+        <v>23</v>
       </c>
       <c r="Q5" s="38"/>
       <c r="R5" s="38"/>
@@ -1968,28 +1970,30 @@
         <v>1</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E6" s="5">
         <v>5</v>
       </c>
-      <c r="F6" s="1"/>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
       <c r="G6" s="1">
-        <v>4</v>
-      </c>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1">
-        <v>-1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="H6" s="1">
+        <v>3</v>
+      </c>
+      <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="6"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="27"/>
-      <c r="P6" s="58" t="str">
+      <c r="P6" s="57" t="str">
         <f>IF(COUNT(E6:O6) = 0,"-",IF(E6&gt;SUM(F6:O6),"Incomplete","Done"))</f>
-        <v>Incomplete</v>
+        <v>Done</v>
       </c>
       <c r="R6" s="14"/>
       <c r="S6" s="33" t="s">
@@ -2024,7 +2028,7 @@
       </c>
       <c r="N7" s="1"/>
       <c r="O7" s="27"/>
-      <c r="P7" s="58" t="str">
+      <c r="P7" s="57" t="str">
         <f t="shared" ref="P7:P25" si="0">IF(COUNT(E7:O7) = 0,"-",IF(E7&gt;SUM(F7:O7),"Incomplete","Done"))</f>
         <v>Done</v>
       </c>
@@ -2044,8 +2048,12 @@
       <c r="D8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="5"/>
+      <c r="E8" s="9">
+        <v>5</v>
+      </c>
+      <c r="F8" s="5">
+        <v>1</v>
+      </c>
       <c r="G8" s="5"/>
       <c r="H8" s="8">
         <v>-3</v>
@@ -2059,9 +2067,9 @@
       </c>
       <c r="N8" s="5"/>
       <c r="O8" s="28"/>
-      <c r="P8" s="58" t="str">
+      <c r="P8" s="57" t="str">
         <f t="shared" si="0"/>
-        <v>Done</v>
+        <v>Incomplete</v>
       </c>
       <c r="R8" s="16"/>
       <c r="S8" s="9"/>
@@ -2095,12 +2103,12 @@
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
       <c r="O9" s="28"/>
-      <c r="P9" s="58" t="str">
+      <c r="P9" s="57" t="str">
         <f t="shared" si="0"/>
         <v>Done</v>
       </c>
       <c r="R9" s="16"/>
-      <c r="S9" s="60"/>
+      <c r="S9" s="59"/>
       <c r="T9" s="13" t="s">
         <v>12</v>
       </c>
@@ -2114,7 +2122,7 @@
         <v>5</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="1"/>
@@ -2131,12 +2139,12 @@
       <c r="O10" s="29">
         <v>3</v>
       </c>
-      <c r="P10" s="58" t="str">
+      <c r="P10" s="57" t="str">
         <f t="shared" si="0"/>
         <v>Done</v>
       </c>
       <c r="R10" s="16"/>
-      <c r="S10" s="61"/>
+      <c r="S10" s="60"/>
       <c r="T10" s="13"/>
       <c r="U10" s="13"/>
       <c r="V10" s="17"/>
@@ -2145,24 +2153,24 @@
     <row r="11" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="36"/>
       <c r="B11" s="16"/>
-      <c r="C11" s="62">
+      <c r="C11" s="61">
         <v>6</v>
       </c>
-      <c r="D11" s="63" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="64"/>
-      <c r="F11" s="64"/>
-      <c r="G11" s="64"/>
-      <c r="H11" s="64"/>
-      <c r="I11" s="64"/>
-      <c r="J11" s="64"/>
-      <c r="K11" s="64"/>
-      <c r="L11" s="64"/>
-      <c r="M11" s="64"/>
-      <c r="N11" s="64"/>
-      <c r="O11" s="65"/>
-      <c r="P11" s="58" t="str">
+      <c r="D11" s="62" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="63"/>
+      <c r="F11" s="63"/>
+      <c r="G11" s="63"/>
+      <c r="H11" s="63"/>
+      <c r="I11" s="63"/>
+      <c r="J11" s="63"/>
+      <c r="K11" s="63"/>
+      <c r="L11" s="63"/>
+      <c r="M11" s="63"/>
+      <c r="N11" s="63"/>
+      <c r="O11" s="64"/>
+      <c r="P11" s="57" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
@@ -2175,12 +2183,12 @@
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" s="36"/>
-      <c r="B12" s="69"/>
-      <c r="C12" s="68">
+      <c r="B12" s="68"/>
+      <c r="C12" s="67">
         <v>7</v>
       </c>
-      <c r="D12" s="63" t="s">
-        <v>27</v>
+      <c r="D12" s="62" t="s">
+        <v>26</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
@@ -2193,7 +2201,7 @@
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
       <c r="O12" s="28"/>
-      <c r="P12" s="58" t="str">
+      <c r="P12" s="57" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
@@ -2201,13 +2209,19 @@
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" s="36"/>
-      <c r="B13" s="69"/>
-      <c r="C13" s="68">
+      <c r="B13" s="68"/>
+      <c r="C13" s="67">
         <v>8</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
+      <c r="D13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="5">
+        <v>5</v>
+      </c>
+      <c r="F13" s="5">
+        <v>-1</v>
+      </c>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
@@ -2217,9 +2231,9 @@
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
       <c r="O13" s="28"/>
-      <c r="P13" s="58" t="str">
+      <c r="P13" s="57" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>Incomplete</v>
       </c>
       <c r="Q13" s="13"/>
       <c r="R13" s="13"/>
@@ -2230,8 +2244,8 @@
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" s="36"/>
-      <c r="B14" s="69"/>
-      <c r="C14" s="68">
+      <c r="B14" s="68"/>
+      <c r="C14" s="67">
         <v>9</v>
       </c>
       <c r="D14" s="4"/>
@@ -2246,7 +2260,7 @@
       <c r="M14" s="5"/>
       <c r="N14" s="5"/>
       <c r="O14" s="28"/>
-      <c r="P14" s="58" t="str">
+      <c r="P14" s="57" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
@@ -2259,8 +2273,8 @@
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" s="36"/>
-      <c r="B15" s="69"/>
-      <c r="C15" s="68">
+      <c r="B15" s="68"/>
+      <c r="C15" s="67">
         <v>10</v>
       </c>
       <c r="D15" s="4"/>
@@ -2275,22 +2289,22 @@
       <c r="M15" s="5"/>
       <c r="N15" s="5"/>
       <c r="O15" s="28"/>
-      <c r="P15" s="58" t="str">
+      <c r="P15" s="57" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="Q15" s="59"/>
-      <c r="R15" s="59"/>
-      <c r="S15" s="59"/>
-      <c r="T15" s="59"/>
-      <c r="U15" s="59"/>
-      <c r="V15" s="59"/>
+      <c r="Q15" s="58"/>
+      <c r="R15" s="58"/>
+      <c r="S15" s="58"/>
+      <c r="T15" s="58"/>
+      <c r="U15" s="58"/>
+      <c r="V15" s="58"/>
       <c r="W15" s="17"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16" s="36"/>
-      <c r="B16" s="69"/>
-      <c r="C16" s="68">
+      <c r="B16" s="68"/>
+      <c r="C16" s="67">
         <v>11</v>
       </c>
       <c r="D16" s="4"/>
@@ -2305,25 +2319,27 @@
       <c r="M16" s="5"/>
       <c r="N16" s="5"/>
       <c r="O16" s="28"/>
-      <c r="P16" s="58" t="str">
+      <c r="P16" s="57" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="Q16" s="59"/>
-      <c r="R16" s="59"/>
-      <c r="S16" s="59"/>
-      <c r="T16" s="59"/>
-      <c r="U16" s="59"/>
-      <c r="V16" s="59"/>
+      <c r="Q16" s="58"/>
+      <c r="R16" s="58"/>
+      <c r="S16" s="58"/>
+      <c r="T16" s="58"/>
+      <c r="U16" s="58"/>
+      <c r="V16" s="58"/>
       <c r="W16" s="17"/>
     </row>
     <row r="17" spans="1:24" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="36"/>
-      <c r="B17" s="69"/>
-      <c r="C17" s="68">
+      <c r="B17" s="68"/>
+      <c r="C17" s="67">
         <v>12</v>
       </c>
-      <c r="D17" s="4"/>
+      <c r="D17" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
@@ -2335,22 +2351,22 @@
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
       <c r="O17" s="28"/>
-      <c r="P17" s="58" t="str">
+      <c r="P17" s="57" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="Q17" s="59"/>
-      <c r="R17" s="59"/>
-      <c r="S17" s="59"/>
-      <c r="T17" s="59"/>
-      <c r="U17" s="59"/>
-      <c r="V17" s="59"/>
+      <c r="Q17" s="58"/>
+      <c r="R17" s="58"/>
+      <c r="S17" s="58"/>
+      <c r="T17" s="58"/>
+      <c r="U17" s="58"/>
+      <c r="V17" s="58"/>
       <c r="W17" s="17"/>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18" s="36"/>
-      <c r="B18" s="69"/>
-      <c r="C18" s="68">
+      <c r="B18" s="68"/>
+      <c r="C18" s="67">
         <v>13</v>
       </c>
       <c r="D18" s="4"/>
@@ -2365,22 +2381,22 @@
       <c r="M18" s="5"/>
       <c r="N18" s="5"/>
       <c r="O18" s="28"/>
-      <c r="P18" s="58" t="str">
+      <c r="P18" s="57" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="Q18" s="59"/>
-      <c r="R18" s="59"/>
-      <c r="S18" s="59"/>
-      <c r="T18" s="59"/>
-      <c r="U18" s="59"/>
-      <c r="V18" s="59"/>
+      <c r="Q18" s="58"/>
+      <c r="R18" s="58"/>
+      <c r="S18" s="58"/>
+      <c r="T18" s="58"/>
+      <c r="U18" s="58"/>
+      <c r="V18" s="58"/>
       <c r="W18" s="17"/>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A19" s="36"/>
-      <c r="B19" s="69"/>
-      <c r="C19" s="68">
+      <c r="B19" s="68"/>
+      <c r="C19" s="67">
         <v>14</v>
       </c>
       <c r="D19" s="4"/>
@@ -2395,22 +2411,22 @@
       <c r="M19" s="5"/>
       <c r="N19" s="5"/>
       <c r="O19" s="28"/>
-      <c r="P19" s="58" t="str">
+      <c r="P19" s="57" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="Q19" s="59"/>
-      <c r="R19" s="59"/>
-      <c r="S19" s="59"/>
-      <c r="T19" s="59"/>
-      <c r="U19" s="59"/>
-      <c r="V19" s="59"/>
+      <c r="Q19" s="58"/>
+      <c r="R19" s="58"/>
+      <c r="S19" s="58"/>
+      <c r="T19" s="58"/>
+      <c r="U19" s="58"/>
+      <c r="V19" s="58"/>
       <c r="W19" s="17"/>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A20" s="36"/>
-      <c r="B20" s="69"/>
-      <c r="C20" s="68">
+      <c r="B20" s="68"/>
+      <c r="C20" s="67">
         <v>15</v>
       </c>
       <c r="D20" s="4"/>
@@ -2425,22 +2441,22 @@
       <c r="M20" s="5"/>
       <c r="N20" s="5"/>
       <c r="O20" s="28"/>
-      <c r="P20" s="58" t="str">
+      <c r="P20" s="57" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="Q20" s="59"/>
-      <c r="R20" s="59"/>
-      <c r="S20" s="59"/>
-      <c r="T20" s="59"/>
-      <c r="U20" s="59"/>
-      <c r="V20" s="59"/>
+      <c r="Q20" s="58"/>
+      <c r="R20" s="58"/>
+      <c r="S20" s="58"/>
+      <c r="T20" s="58"/>
+      <c r="U20" s="58"/>
+      <c r="V20" s="58"/>
       <c r="W20" s="17"/>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A21" s="36"/>
-      <c r="B21" s="69"/>
-      <c r="C21" s="68">
+      <c r="B21" s="68"/>
+      <c r="C21" s="67">
         <v>16</v>
       </c>
       <c r="D21" s="4"/>
@@ -2455,22 +2471,22 @@
       <c r="M21" s="5"/>
       <c r="N21" s="5"/>
       <c r="O21" s="28"/>
-      <c r="P21" s="58" t="str">
+      <c r="P21" s="57" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="Q21" s="59"/>
-      <c r="R21" s="59"/>
-      <c r="S21" s="59"/>
-      <c r="T21" s="59"/>
-      <c r="U21" s="59"/>
-      <c r="V21" s="59"/>
+      <c r="Q21" s="58"/>
+      <c r="R21" s="58"/>
+      <c r="S21" s="58"/>
+      <c r="T21" s="58"/>
+      <c r="U21" s="58"/>
+      <c r="V21" s="58"/>
       <c r="W21" s="17"/>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A22" s="36"/>
-      <c r="B22" s="69"/>
-      <c r="C22" s="68">
+      <c r="B22" s="68"/>
+      <c r="C22" s="67">
         <v>17</v>
       </c>
       <c r="D22" s="4"/>
@@ -2485,22 +2501,22 @@
       <c r="M22" s="5"/>
       <c r="N22" s="5"/>
       <c r="O22" s="28"/>
-      <c r="P22" s="58" t="str">
+      <c r="P22" s="57" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="Q22" s="59"/>
-      <c r="R22" s="59"/>
-      <c r="S22" s="59"/>
-      <c r="T22" s="59"/>
-      <c r="U22" s="59"/>
-      <c r="V22" s="59"/>
+      <c r="Q22" s="58"/>
+      <c r="R22" s="58"/>
+      <c r="S22" s="58"/>
+      <c r="T22" s="58"/>
+      <c r="U22" s="58"/>
+      <c r="V22" s="58"/>
       <c r="W22" s="17"/>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A23" s="36"/>
-      <c r="B23" s="69"/>
-      <c r="C23" s="68">
+      <c r="B23" s="68"/>
+      <c r="C23" s="67">
         <v>18</v>
       </c>
       <c r="D23" s="4"/>
@@ -2515,22 +2531,22 @@
       <c r="M23" s="5"/>
       <c r="N23" s="5"/>
       <c r="O23" s="28"/>
-      <c r="P23" s="58" t="str">
+      <c r="P23" s="57" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="Q23" s="59"/>
-      <c r="R23" s="59"/>
-      <c r="S23" s="59"/>
-      <c r="T23" s="59"/>
-      <c r="U23" s="59"/>
-      <c r="V23" s="59"/>
+      <c r="Q23" s="58"/>
+      <c r="R23" s="58"/>
+      <c r="S23" s="58"/>
+      <c r="T23" s="58"/>
+      <c r="U23" s="58"/>
+      <c r="V23" s="58"/>
       <c r="W23" s="17"/>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A24" s="36"/>
-      <c r="B24" s="69"/>
-      <c r="C24" s="68">
+      <c r="B24" s="68"/>
+      <c r="C24" s="67">
         <v>19</v>
       </c>
       <c r="D24" s="4"/>
@@ -2545,22 +2561,22 @@
       <c r="M24" s="5"/>
       <c r="N24" s="5"/>
       <c r="O24" s="28"/>
-      <c r="P24" s="58" t="str">
+      <c r="P24" s="57" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="Q24" s="59"/>
-      <c r="R24" s="59"/>
-      <c r="S24" s="59"/>
-      <c r="T24" s="59"/>
-      <c r="U24" s="59"/>
-      <c r="V24" s="59"/>
+      <c r="Q24" s="58"/>
+      <c r="R24" s="58"/>
+      <c r="S24" s="58"/>
+      <c r="T24" s="58"/>
+      <c r="U24" s="58"/>
+      <c r="V24" s="58"/>
       <c r="W24" s="17"/>
     </row>
     <row r="25" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="36"/>
-      <c r="B25" s="69"/>
-      <c r="C25" s="68">
+      <c r="B25" s="68"/>
+      <c r="C25" s="67">
         <v>20</v>
       </c>
       <c r="D25" s="4"/>
@@ -2575,16 +2591,16 @@
       <c r="M25" s="30"/>
       <c r="N25" s="30"/>
       <c r="O25" s="32"/>
-      <c r="P25" s="58" t="str">
+      <c r="P25" s="57" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="Q25" s="59"/>
-      <c r="R25" s="59"/>
-      <c r="S25" s="59"/>
-      <c r="T25" s="59"/>
-      <c r="U25" s="59"/>
-      <c r="V25" s="59"/>
+      <c r="Q25" s="58"/>
+      <c r="R25" s="58"/>
+      <c r="S25" s="58"/>
+      <c r="T25" s="58"/>
+      <c r="U25" s="58"/>
+      <c r="V25" s="58"/>
       <c r="W25" s="17"/>
     </row>
     <row r="26" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2592,169 +2608,169 @@
       <c r="B26" s="16"/>
       <c r="C26" s="48"/>
       <c r="D26" s="40" t="s">
-        <v>23</v>
-      </c>
-      <c r="E26" s="66">
-        <f>SUM(E6:E12)</f>
-        <v>7</v>
-      </c>
-      <c r="F26" s="67">
-        <f t="shared" ref="F26:O26" si="1">E26-SUM(F6:F12)</f>
-        <v>7</v>
-      </c>
-      <c r="G26" s="67">
+        <v>22</v>
+      </c>
+      <c r="E26" s="65">
+        <f>SUM(E6:E20)</f>
+        <v>17</v>
+      </c>
+      <c r="F26" s="66">
+        <f>E26-SUM(F6:F20)</f>
+        <v>16</v>
+      </c>
+      <c r="G26" s="66">
+        <f t="shared" ref="G26:O26" si="1">F26-SUM(G6:G20)</f>
+        <v>15</v>
+      </c>
+      <c r="H26" s="66">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="H26" s="67">
+        <v>15</v>
+      </c>
+      <c r="I26" s="66">
         <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="I26" s="67">
+        <v>15</v>
+      </c>
+      <c r="J26" s="66">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="J26" s="67">
+        <v>17</v>
+      </c>
+      <c r="K26" s="66">
         <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="K26" s="67">
+        <v>20</v>
+      </c>
+      <c r="L26" s="66">
         <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="L26" s="67">
+        <v>18</v>
+      </c>
+      <c r="M26" s="66">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="N26" s="66">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="O26" s="66">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="M26" s="67">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="N26" s="67">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="O26" s="50">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="P26" s="70"/>
-      <c r="Q26" s="59"/>
-      <c r="R26" s="59"/>
-      <c r="S26" s="59"/>
-      <c r="T26" s="59"/>
-      <c r="U26" s="59"/>
-      <c r="V26" s="59"/>
+      <c r="P26" s="69"/>
+      <c r="Q26" s="58"/>
+      <c r="R26" s="58"/>
+      <c r="S26" s="58"/>
+      <c r="T26" s="58"/>
+      <c r="U26" s="58"/>
+      <c r="V26" s="58"/>
       <c r="W26" s="17"/>
     </row>
     <row r="27" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="36"/>
       <c r="B27" s="16"/>
       <c r="C27" s="49"/>
-      <c r="D27" s="51" t="s">
+      <c r="D27" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="E27" s="52">
+      <c r="E27" s="51">
         <f>E26</f>
-        <v>7</v>
-      </c>
-      <c r="F27" s="53">
+        <v>17</v>
+      </c>
+      <c r="F27" s="52">
         <f t="shared" ref="F27:O27" si="2">E27-($E$26/10)</f>
-        <v>6.3</v>
-      </c>
-      <c r="G27" s="53">
+        <v>15.3</v>
+      </c>
+      <c r="G27" s="52">
         <f t="shared" si="2"/>
-        <v>5.6</v>
-      </c>
-      <c r="H27" s="53">
+        <v>13.600000000000001</v>
+      </c>
+      <c r="H27" s="52">
         <f t="shared" si="2"/>
-        <v>4.8999999999999995</v>
-      </c>
-      <c r="I27" s="53">
+        <v>11.900000000000002</v>
+      </c>
+      <c r="I27" s="52">
         <f t="shared" si="2"/>
-        <v>4.1999999999999993</v>
-      </c>
-      <c r="J27" s="53">
+        <v>10.200000000000003</v>
+      </c>
+      <c r="J27" s="52">
         <f t="shared" si="2"/>
-        <v>3.4999999999999991</v>
-      </c>
-      <c r="K27" s="53">
+        <v>8.5000000000000036</v>
+      </c>
+      <c r="K27" s="52">
         <f t="shared" si="2"/>
-        <v>2.7999999999999989</v>
-      </c>
-      <c r="L27" s="53">
+        <v>6.8000000000000034</v>
+      </c>
+      <c r="L27" s="52">
         <f t="shared" si="2"/>
-        <v>2.0999999999999988</v>
-      </c>
-      <c r="M27" s="53">
+        <v>5.1000000000000032</v>
+      </c>
+      <c r="M27" s="52">
         <f t="shared" si="2"/>
-        <v>1.3999999999999988</v>
-      </c>
-      <c r="N27" s="53">
+        <v>3.400000000000003</v>
+      </c>
+      <c r="N27" s="52">
         <f t="shared" si="2"/>
-        <v>0.69999999999999885</v>
-      </c>
-      <c r="O27" s="54">
+        <v>1.7000000000000031</v>
+      </c>
+      <c r="O27" s="53">
         <f t="shared" si="2"/>
-        <v>-1.1102230246251565E-15</v>
-      </c>
-      <c r="P27" s="59"/>
-      <c r="Q27" s="59"/>
-      <c r="R27" s="59"/>
-      <c r="S27" s="59"/>
-      <c r="T27" s="59"/>
-      <c r="U27" s="59"/>
-      <c r="V27" s="59"/>
+        <v>3.1086244689504383E-15</v>
+      </c>
+      <c r="P27" s="58"/>
+      <c r="Q27" s="58"/>
+      <c r="R27" s="58"/>
+      <c r="S27" s="58"/>
+      <c r="T27" s="58"/>
+      <c r="U27" s="58"/>
+      <c r="V27" s="58"/>
       <c r="W27" s="17"/>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A28" s="36"/>
       <c r="B28" s="16"/>
-      <c r="C28" s="59"/>
-      <c r="D28" s="59"/>
-      <c r="E28" s="59"/>
-      <c r="F28" s="59"/>
-      <c r="G28" s="59"/>
-      <c r="H28" s="59"/>
-      <c r="I28" s="59"/>
-      <c r="J28" s="59"/>
-      <c r="K28" s="59"/>
-      <c r="L28" s="59"/>
-      <c r="M28" s="59"/>
-      <c r="N28" s="59"/>
-      <c r="O28" s="59"/>
-      <c r="P28" s="59"/>
-      <c r="Q28" s="59"/>
-      <c r="R28" s="59"/>
-      <c r="S28" s="59"/>
-      <c r="T28" s="59"/>
-      <c r="U28" s="59"/>
-      <c r="V28" s="59"/>
+      <c r="C28" s="58"/>
+      <c r="D28" s="58"/>
+      <c r="E28" s="58"/>
+      <c r="F28" s="58"/>
+      <c r="G28" s="58"/>
+      <c r="H28" s="58"/>
+      <c r="I28" s="58"/>
+      <c r="J28" s="58"/>
+      <c r="K28" s="58"/>
+      <c r="L28" s="58"/>
+      <c r="M28" s="58"/>
+      <c r="N28" s="58"/>
+      <c r="O28" s="58"/>
+      <c r="P28" s="58"/>
+      <c r="Q28" s="58"/>
+      <c r="R28" s="58"/>
+      <c r="S28" s="58"/>
+      <c r="T28" s="58"/>
+      <c r="U28" s="58"/>
+      <c r="V28" s="58"/>
       <c r="W28" s="17"/>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A29" s="36"/>
       <c r="B29" s="16"/>
-      <c r="C29" s="59"/>
-      <c r="D29" s="59"/>
-      <c r="E29" s="59"/>
-      <c r="F29" s="59"/>
-      <c r="G29" s="59"/>
-      <c r="H29" s="59"/>
-      <c r="I29" s="59"/>
-      <c r="J29" s="59"/>
-      <c r="K29" s="59"/>
-      <c r="L29" s="59"/>
-      <c r="M29" s="59"/>
-      <c r="N29" s="59"/>
-      <c r="O29" s="59"/>
-      <c r="P29" s="59"/>
-      <c r="Q29" s="59"/>
-      <c r="R29" s="59"/>
-      <c r="S29" s="59"/>
-      <c r="T29" s="59"/>
-      <c r="U29" s="59"/>
-      <c r="V29" s="59"/>
+      <c r="C29" s="58"/>
+      <c r="D29" s="58"/>
+      <c r="E29" s="58"/>
+      <c r="F29" s="58"/>
+      <c r="G29" s="58"/>
+      <c r="H29" s="58"/>
+      <c r="I29" s="58"/>
+      <c r="J29" s="58"/>
+      <c r="K29" s="58"/>
+      <c r="L29" s="58"/>
+      <c r="M29" s="58"/>
+      <c r="N29" s="58"/>
+      <c r="O29" s="58"/>
+      <c r="P29" s="58"/>
+      <c r="Q29" s="58"/>
+      <c r="R29" s="58"/>
+      <c r="S29" s="58"/>
+      <c r="T29" s="58"/>
+      <c r="U29" s="58"/>
+      <c r="V29" s="58"/>
       <c r="W29" s="17"/>
     </row>
     <row r="30" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2779,7 +2795,7 @@
       <c r="S30" s="19"/>
       <c r="T30" s="19"/>
       <c r="U30" s="19"/>
-      <c r="V30" s="55"/>
+      <c r="V30" s="54"/>
       <c r="W30" s="20"/>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.3">
@@ -2801,130 +2817,130 @@
     <row r="35" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A35" s="36"/>
       <c r="B35" s="13"/>
-      <c r="C35" s="59"/>
-      <c r="D35" s="59"/>
-      <c r="E35" s="59"/>
-      <c r="F35" s="59"/>
-      <c r="G35" s="59"/>
-      <c r="H35" s="59"/>
-      <c r="I35" s="59"/>
-      <c r="J35" s="59"/>
-      <c r="K35" s="59"/>
-      <c r="L35" s="59"/>
-      <c r="M35" s="59"/>
-      <c r="N35" s="59"/>
-      <c r="O35" s="59"/>
-      <c r="P35" s="59"/>
-      <c r="Q35" s="59"/>
-      <c r="R35" s="59"/>
-      <c r="S35" s="59"/>
-      <c r="T35" s="59"/>
-      <c r="U35" s="59"/>
-      <c r="V35" s="59"/>
+      <c r="C35" s="58"/>
+      <c r="D35" s="58"/>
+      <c r="E35" s="58"/>
+      <c r="F35" s="58"/>
+      <c r="G35" s="58"/>
+      <c r="H35" s="58"/>
+      <c r="I35" s="58"/>
+      <c r="J35" s="58"/>
+      <c r="K35" s="58"/>
+      <c r="L35" s="58"/>
+      <c r="M35" s="58"/>
+      <c r="N35" s="58"/>
+      <c r="O35" s="58"/>
+      <c r="P35" s="58"/>
+      <c r="Q35" s="58"/>
+      <c r="R35" s="58"/>
+      <c r="S35" s="58"/>
+      <c r="T35" s="58"/>
+      <c r="U35" s="58"/>
+      <c r="V35" s="58"/>
       <c r="W35" s="13"/>
       <c r="X35" s="23"/>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A36" s="36"/>
       <c r="B36" s="13"/>
-      <c r="C36" s="59"/>
-      <c r="D36" s="59"/>
-      <c r="E36" s="59"/>
-      <c r="F36" s="59"/>
-      <c r="G36" s="59"/>
-      <c r="H36" s="59"/>
-      <c r="I36" s="59"/>
-      <c r="J36" s="59"/>
-      <c r="K36" s="59"/>
-      <c r="L36" s="59"/>
-      <c r="M36" s="59"/>
-      <c r="N36" s="59"/>
-      <c r="O36" s="59"/>
-      <c r="P36" s="59"/>
-      <c r="Q36" s="59"/>
-      <c r="R36" s="59"/>
-      <c r="S36" s="59"/>
-      <c r="T36" s="59"/>
-      <c r="U36" s="59"/>
-      <c r="V36" s="59"/>
+      <c r="C36" s="58"/>
+      <c r="D36" s="58"/>
+      <c r="E36" s="58"/>
+      <c r="F36" s="58"/>
+      <c r="G36" s="58"/>
+      <c r="H36" s="58"/>
+      <c r="I36" s="58"/>
+      <c r="J36" s="58"/>
+      <c r="K36" s="58"/>
+      <c r="L36" s="58"/>
+      <c r="M36" s="58"/>
+      <c r="N36" s="58"/>
+      <c r="O36" s="58"/>
+      <c r="P36" s="58"/>
+      <c r="Q36" s="58"/>
+      <c r="R36" s="58"/>
+      <c r="S36" s="58"/>
+      <c r="T36" s="58"/>
+      <c r="U36" s="58"/>
+      <c r="V36" s="58"/>
       <c r="W36" s="13"/>
       <c r="X36" s="23"/>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A37" s="36"/>
       <c r="B37" s="13"/>
-      <c r="C37" s="59"/>
-      <c r="D37" s="59"/>
-      <c r="E37" s="59"/>
-      <c r="F37" s="59"/>
-      <c r="G37" s="59"/>
-      <c r="H37" s="59"/>
-      <c r="I37" s="59"/>
-      <c r="J37" s="59"/>
-      <c r="K37" s="59"/>
-      <c r="L37" s="59"/>
-      <c r="M37" s="59"/>
-      <c r="N37" s="59"/>
-      <c r="O37" s="59"/>
-      <c r="P37" s="59"/>
-      <c r="Q37" s="59"/>
-      <c r="R37" s="59"/>
-      <c r="S37" s="59"/>
-      <c r="T37" s="59"/>
-      <c r="U37" s="59"/>
-      <c r="V37" s="59"/>
+      <c r="C37" s="58"/>
+      <c r="D37" s="58"/>
+      <c r="E37" s="58"/>
+      <c r="F37" s="58"/>
+      <c r="G37" s="58"/>
+      <c r="H37" s="58"/>
+      <c r="I37" s="58"/>
+      <c r="J37" s="58"/>
+      <c r="K37" s="58"/>
+      <c r="L37" s="58"/>
+      <c r="M37" s="58"/>
+      <c r="N37" s="58"/>
+      <c r="O37" s="58"/>
+      <c r="P37" s="58"/>
+      <c r="Q37" s="58"/>
+      <c r="R37" s="58"/>
+      <c r="S37" s="58"/>
+      <c r="T37" s="58"/>
+      <c r="U37" s="58"/>
+      <c r="V37" s="58"/>
       <c r="W37" s="13"/>
       <c r="X37" s="23"/>
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A38" s="36"/>
       <c r="B38" s="13"/>
-      <c r="C38" s="59"/>
-      <c r="D38" s="59"/>
-      <c r="E38" s="59"/>
-      <c r="F38" s="59"/>
-      <c r="G38" s="59"/>
-      <c r="H38" s="59"/>
-      <c r="I38" s="59"/>
-      <c r="J38" s="59"/>
-      <c r="K38" s="59"/>
-      <c r="L38" s="59"/>
-      <c r="M38" s="59"/>
-      <c r="N38" s="59"/>
-      <c r="O38" s="59"/>
-      <c r="P38" s="59"/>
-      <c r="Q38" s="59"/>
-      <c r="R38" s="59"/>
-      <c r="S38" s="59"/>
-      <c r="T38" s="59"/>
-      <c r="U38" s="59"/>
-      <c r="V38" s="59"/>
+      <c r="C38" s="58"/>
+      <c r="D38" s="58"/>
+      <c r="E38" s="58"/>
+      <c r="F38" s="58"/>
+      <c r="G38" s="58"/>
+      <c r="H38" s="58"/>
+      <c r="I38" s="58"/>
+      <c r="J38" s="58"/>
+      <c r="K38" s="58"/>
+      <c r="L38" s="58"/>
+      <c r="M38" s="58"/>
+      <c r="N38" s="58"/>
+      <c r="O38" s="58"/>
+      <c r="P38" s="58"/>
+      <c r="Q38" s="58"/>
+      <c r="R38" s="58"/>
+      <c r="S38" s="58"/>
+      <c r="T38" s="58"/>
+      <c r="U38" s="58"/>
+      <c r="V38" s="58"/>
       <c r="W38" s="13"/>
       <c r="X38" s="23"/>
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A39" s="36"/>
       <c r="B39" s="13"/>
-      <c r="C39" s="59"/>
-      <c r="D39" s="59"/>
-      <c r="E39" s="59"/>
-      <c r="F39" s="59"/>
-      <c r="G39" s="59"/>
-      <c r="H39" s="59"/>
-      <c r="I39" s="59"/>
-      <c r="J39" s="59"/>
-      <c r="K39" s="59"/>
-      <c r="L39" s="59"/>
-      <c r="M39" s="59"/>
-      <c r="N39" s="59"/>
-      <c r="O39" s="59"/>
-      <c r="P39" s="59"/>
-      <c r="Q39" s="59"/>
-      <c r="R39" s="59"/>
-      <c r="S39" s="59"/>
-      <c r="T39" s="59"/>
-      <c r="U39" s="59"/>
-      <c r="V39" s="59"/>
+      <c r="C39" s="58"/>
+      <c r="D39" s="58"/>
+      <c r="E39" s="58"/>
+      <c r="F39" s="58"/>
+      <c r="G39" s="58"/>
+      <c r="H39" s="58"/>
+      <c r="I39" s="58"/>
+      <c r="J39" s="58"/>
+      <c r="K39" s="58"/>
+      <c r="L39" s="58"/>
+      <c r="M39" s="58"/>
+      <c r="N39" s="58"/>
+      <c r="O39" s="58"/>
+      <c r="P39" s="58"/>
+      <c r="Q39" s="58"/>
+      <c r="R39" s="58"/>
+      <c r="S39" s="58"/>
+      <c r="T39" s="58"/>
+      <c r="U39" s="58"/>
+      <c r="V39" s="58"/>
       <c r="W39" s="13"/>
       <c r="X39" s="23"/>
     </row>
@@ -2999,14 +3015,18 @@
       <formula>NOT(ISERROR(SEARCH("Done",P6)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S8 E6:E25">
+  <dataValidations count="3">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S8">
       <formula1>0</formula1>
       <formula2>1000000</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O12 L12 S9:S10 F6:K25 L6:O11 O14 O16 O18 O20 O22 O24 L14 L16 L18 L20 L22 L24 L13:O13 L15:O15 L17:O17 L19:O19 L21:O21 L23:O23 L25:O25">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S9:S10">
       <formula1>-100</formula1>
       <formula2>1000000</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6:O27">
+      <formula1>-24</formula1>
+      <formula2>24</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
"Updated SprintBurnDown and Started LOG_IN Scenario from Salonika"
</commit_message>
<xml_diff>
--- a/Done/Sprint_Burndown_Chart_Template.xlsx
+++ b/Done/Sprint_Burndown_Chart_Template.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bbui1\Documents\GitHub\swe443\SWE443BankSystemBlue\Done\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Salonika/Desktop/GitRepo/SWE443BankSystemBlue/Done/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24600" windowHeight="14700"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown Chart Template" sheetId="5" r:id="rId1"/>
@@ -20,7 +20,15 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Burndown Chart Template'!$B$31:$V$40</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Burndown Chart Template'!$3:$5</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -30,7 +38,7 @@
     <author>Anne</author>
   </authors>
   <commentList>
-    <comment ref="E5" authorId="0" shapeId="0">
+    <comment ref="E5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -54,7 +62,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G6" authorId="0" shapeId="0">
+    <comment ref="G6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -78,7 +86,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H8" authorId="0" shapeId="0">
+    <comment ref="H8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -102,7 +110,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S8" authorId="0" shapeId="0">
+    <comment ref="S8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -116,7 +124,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J9" authorId="0" shapeId="0">
+    <comment ref="J9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -140,7 +148,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L9" authorId="0" shapeId="0">
+    <comment ref="L9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -165,7 +173,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S9" authorId="0" shapeId="0">
+    <comment ref="S9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -179,7 +187,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K10" authorId="0" shapeId="0">
+    <comment ref="K10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -193,7 +201,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O10" authorId="0" shapeId="0">
+    <comment ref="O10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -207,7 +215,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P10" authorId="0" shapeId="0">
+    <comment ref="P10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -319,7 +327,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -495,25 +503,25 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -522,20 +530,20 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -543,24 +551,24 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -569,7 +577,7 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -577,17 +585,17 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -597,7 +605,7 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -605,12 +613,12 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -619,27 +627,27 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -647,99 +655,99 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -747,78 +755,78 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -826,13 +834,13 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -841,60 +849,60 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1099,7 +1107,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1128,6 +1136,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1172,8 +1181,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -1185,43 +1195,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>17</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16</c:v>
+                  <c:v>19.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>20</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>18</c:v>
+                  <c:v>21.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>13</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>13</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-89B2-4689-9D60-2A49D583E5FD}"/>
             </c:ext>
@@ -1260,43 +1270,43 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>17</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15.3</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13.600000000000001</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.900000000000002</c:v>
+                  <c:v>14.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10.200000000000003</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.5000000000000036</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.8000000000000034</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.1000000000000032</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.400000000000003</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.7000000000000031</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.1086244689504383E-15</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-89B2-4689-9D60-2A49D583E5FD}"/>
             </c:ext>
@@ -1311,11 +1321,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="414553768"/>
-        <c:axId val="414555728"/>
+        <c:axId val="998835584"/>
+        <c:axId val="957046880"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="414553768"/>
+        <c:axId val="998835584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1325,7 +1335,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="414555728"/>
+        <c:crossAx val="957046880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1333,7 +1343,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="414555728"/>
+        <c:axId val="957046880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1344,13 +1354,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="414553768"/>
+        <c:crossAx val="998835584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -1424,7 +1435,7 @@
         <xdr:cNvPr id="9230" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E240000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000E240000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1493,9 +1504,9 @@
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -1523,31 +1534,14 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -1575,23 +1569,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1768,27 +1745,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="8" tint="0.79998168889431442"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:X42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="131" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="66.5546875" customWidth="1"/>
+    <col min="4" max="4" width="66.5" customWidth="1"/>
     <col min="5" max="15" width="10.6640625" customWidth="1"/>
     <col min="16" max="16" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10.6640625" customWidth="1"/>
-    <col min="24" max="24" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="25.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="49.8" x14ac:dyDescent="0.8">
+    <row r="1" spans="1:23" ht="50" x14ac:dyDescent="0.5">
       <c r="A1" s="36"/>
       <c r="B1" s="76" t="s">
         <v>24</v>
@@ -1815,7 +1792,7 @@
       <c r="V1" s="76"/>
       <c r="W1" s="76"/>
     </row>
-    <row r="2" spans="1:23" ht="33" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:23" ht="34" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="36"/>
       <c r="B2" s="77" t="s">
         <v>21</v>
@@ -1842,7 +1819,7 @@
       <c r="V2" s="77"/>
       <c r="W2" s="77"/>
     </row>
-    <row r="3" spans="1:23" s="2" customFormat="1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:23" s="2" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="34"/>
       <c r="B3" s="41"/>
       <c r="C3" s="42"/>
@@ -1867,7 +1844,7 @@
       <c r="V3" s="70"/>
       <c r="W3" s="44"/>
     </row>
-    <row r="4" spans="1:23" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A4" s="35"/>
       <c r="B4" s="37"/>
       <c r="C4" s="45" t="s">
@@ -1915,7 +1892,7 @@
       <c r="U4" s="38"/>
       <c r="W4" s="39"/>
     </row>
-    <row r="5" spans="1:23" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:23" s="3" customFormat="1" ht="31" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="35"/>
       <c r="B5" s="37"/>
       <c r="C5" s="25"/>
@@ -1963,7 +1940,7 @@
       <c r="U5" s="38"/>
       <c r="W5" s="39"/>
     </row>
-    <row r="6" spans="1:23" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:23" ht="34.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="36"/>
       <c r="B6" s="16"/>
       <c r="C6" s="26">
@@ -2004,7 +1981,7 @@
       <c r="V6" s="15"/>
       <c r="W6" s="17"/>
     </row>
-    <row r="7" spans="1:23" ht="18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:23" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" s="36"/>
       <c r="B7" s="16"/>
       <c r="C7" s="26">
@@ -2039,7 +2016,7 @@
       <c r="V7" s="17"/>
       <c r="W7" s="17"/>
     </row>
-    <row r="8" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="36"/>
       <c r="B8" s="16"/>
       <c r="C8" s="26">
@@ -2079,7 +2056,7 @@
       <c r="V8" s="17"/>
       <c r="W8" s="17"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" s="36"/>
       <c r="B9" s="16"/>
       <c r="C9" s="26">
@@ -2115,7 +2092,7 @@
       <c r="V9" s="17"/>
       <c r="W9" s="17"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" s="36"/>
       <c r="B10" s="16"/>
       <c r="C10" s="26">
@@ -2150,7 +2127,7 @@
       <c r="V10" s="17"/>
       <c r="W10" s="17"/>
     </row>
-    <row r="11" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="36"/>
       <c r="B11" s="16"/>
       <c r="C11" s="61">
@@ -2181,7 +2158,7 @@
       <c r="V11" s="20"/>
       <c r="W11" s="17"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" s="36"/>
       <c r="B12" s="68"/>
       <c r="C12" s="67">
@@ -2207,7 +2184,7 @@
       </c>
       <c r="W12" s="17"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" s="36"/>
       <c r="B13" s="68"/>
       <c r="C13" s="67">
@@ -2242,7 +2219,7 @@
       <c r="U13" s="13"/>
       <c r="W13" s="17"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" s="36"/>
       <c r="B14" s="68"/>
       <c r="C14" s="67">
@@ -2271,7 +2248,7 @@
       <c r="U14" s="13"/>
       <c r="W14" s="17"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" s="36"/>
       <c r="B15" s="68"/>
       <c r="C15" s="67">
@@ -2301,7 +2278,7 @@
       <c r="V15" s="58"/>
       <c r="W15" s="17"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" s="36"/>
       <c r="B16" s="68"/>
       <c r="C16" s="67">
@@ -2331,7 +2308,7 @@
       <c r="V16" s="58"/>
       <c r="W16" s="17"/>
     </row>
-    <row r="17" spans="1:24" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="36"/>
       <c r="B17" s="68"/>
       <c r="C17" s="67">
@@ -2340,7 +2317,9 @@
       <c r="D17" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E17" s="5"/>
+      <c r="E17" s="5">
+        <v>3</v>
+      </c>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
@@ -2353,7 +2332,7 @@
       <c r="O17" s="28"/>
       <c r="P17" s="57" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>Incomplete</v>
       </c>
       <c r="Q17" s="58"/>
       <c r="R17" s="58"/>
@@ -2363,7 +2342,7 @@
       <c r="V17" s="58"/>
       <c r="W17" s="17"/>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18" s="36"/>
       <c r="B18" s="68"/>
       <c r="C18" s="67">
@@ -2393,7 +2372,7 @@
       <c r="V18" s="58"/>
       <c r="W18" s="17"/>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
       <c r="B19" s="68"/>
       <c r="C19" s="67">
@@ -2423,7 +2402,7 @@
       <c r="V19" s="58"/>
       <c r="W19" s="17"/>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20" s="36"/>
       <c r="B20" s="68"/>
       <c r="C20" s="67">
@@ -2453,7 +2432,7 @@
       <c r="V20" s="58"/>
       <c r="W20" s="17"/>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21" s="36"/>
       <c r="B21" s="68"/>
       <c r="C21" s="67">
@@ -2483,7 +2462,7 @@
       <c r="V21" s="58"/>
       <c r="W21" s="17"/>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22" s="36"/>
       <c r="B22" s="68"/>
       <c r="C22" s="67">
@@ -2513,7 +2492,7 @@
       <c r="V22" s="58"/>
       <c r="W22" s="17"/>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A23" s="36"/>
       <c r="B23" s="68"/>
       <c r="C23" s="67">
@@ -2543,7 +2522,7 @@
       <c r="V23" s="58"/>
       <c r="W23" s="17"/>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24" s="36"/>
       <c r="B24" s="68"/>
       <c r="C24" s="67">
@@ -2573,7 +2552,7 @@
       <c r="V24" s="58"/>
       <c r="W24" s="17"/>
     </row>
-    <row r="25" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="36"/>
       <c r="B25" s="68"/>
       <c r="C25" s="67">
@@ -2603,7 +2582,7 @@
       <c r="V25" s="58"/>
       <c r="W25" s="17"/>
     </row>
-    <row r="26" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="36"/>
       <c r="B26" s="16"/>
       <c r="C26" s="48"/>
@@ -2612,47 +2591,47 @@
       </c>
       <c r="E26" s="65">
         <f>SUM(E6:E20)</f>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F26" s="66">
         <f>E26-SUM(F6:F20)</f>
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G26" s="66">
         <f t="shared" ref="G26:O26" si="1">F26-SUM(G6:G20)</f>
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="H26" s="66">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I26" s="66">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="J26" s="66">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="K26" s="66">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="L26" s="66">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="M26" s="66">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="N26" s="66">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="O26" s="66">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="P26" s="69"/>
       <c r="Q26" s="58"/>
@@ -2663,7 +2642,7 @@
       <c r="V26" s="58"/>
       <c r="W26" s="17"/>
     </row>
-    <row r="27" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="36"/>
       <c r="B27" s="16"/>
       <c r="C27" s="49"/>
@@ -2672,47 +2651,47 @@
       </c>
       <c r="E27" s="51">
         <f>E26</f>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F27" s="52">
         <f t="shared" ref="F27:O27" si="2">E27-($E$26/10)</f>
-        <v>15.3</v>
+        <v>18</v>
       </c>
       <c r="G27" s="52">
         <f t="shared" si="2"/>
-        <v>13.600000000000001</v>
+        <v>16</v>
       </c>
       <c r="H27" s="52">
         <f t="shared" si="2"/>
-        <v>11.900000000000002</v>
+        <v>14</v>
       </c>
       <c r="I27" s="52">
         <f t="shared" si="2"/>
-        <v>10.200000000000003</v>
+        <v>12</v>
       </c>
       <c r="J27" s="52">
         <f t="shared" si="2"/>
-        <v>8.5000000000000036</v>
+        <v>10</v>
       </c>
       <c r="K27" s="52">
         <f t="shared" si="2"/>
-        <v>6.8000000000000034</v>
+        <v>8</v>
       </c>
       <c r="L27" s="52">
         <f t="shared" si="2"/>
-        <v>5.1000000000000032</v>
+        <v>6</v>
       </c>
       <c r="M27" s="52">
         <f t="shared" si="2"/>
-        <v>3.400000000000003</v>
+        <v>4</v>
       </c>
       <c r="N27" s="52">
         <f t="shared" si="2"/>
-        <v>1.7000000000000031</v>
+        <v>2</v>
       </c>
       <c r="O27" s="53">
         <f t="shared" si="2"/>
-        <v>3.1086244689504383E-15</v>
+        <v>0</v>
       </c>
       <c r="P27" s="58"/>
       <c r="Q27" s="58"/>
@@ -2723,7 +2702,7 @@
       <c r="V27" s="58"/>
       <c r="W27" s="17"/>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A28" s="36"/>
       <c r="B28" s="16"/>
       <c r="C28" s="58"/>
@@ -2748,7 +2727,7 @@
       <c r="V28" s="58"/>
       <c r="W28" s="17"/>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A29" s="36"/>
       <c r="B29" s="16"/>
       <c r="C29" s="58"/>
@@ -2773,7 +2752,7 @@
       <c r="V29" s="58"/>
       <c r="W29" s="17"/>
     </row>
-    <row r="30" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="36"/>
       <c r="B30" s="18"/>
       <c r="C30" s="19"/>
@@ -2798,23 +2777,23 @@
       <c r="V30" s="54"/>
       <c r="W30" s="20"/>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A31" s="36"/>
       <c r="X31" s="23"/>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A32" s="36"/>
       <c r="X32" s="23"/>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A33" s="36"/>
       <c r="X33" s="23"/>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A34" s="36"/>
       <c r="X34" s="23"/>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A35" s="36"/>
       <c r="B35" s="13"/>
       <c r="C35" s="58"/>
@@ -2840,7 +2819,7 @@
       <c r="W35" s="13"/>
       <c r="X35" s="23"/>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A36" s="36"/>
       <c r="B36" s="13"/>
       <c r="C36" s="58"/>
@@ -2866,7 +2845,7 @@
       <c r="W36" s="13"/>
       <c r="X36" s="23"/>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A37" s="36"/>
       <c r="B37" s="13"/>
       <c r="C37" s="58"/>
@@ -2892,7 +2871,7 @@
       <c r="W37" s="13"/>
       <c r="X37" s="23"/>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A38" s="36"/>
       <c r="B38" s="13"/>
       <c r="C38" s="58"/>
@@ -2918,7 +2897,7 @@
       <c r="W38" s="13"/>
       <c r="X38" s="23"/>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A39" s="36"/>
       <c r="B39" s="13"/>
       <c r="C39" s="58"/>
@@ -2944,7 +2923,7 @@
       <c r="W39" s="13"/>
       <c r="X39" s="23"/>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A40" s="36"/>
       <c r="B40" s="13"/>
       <c r="C40" s="13"/>
@@ -2969,11 +2948,11 @@
       <c r="W40" s="13"/>
       <c r="X40" s="23"/>
     </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A41" s="36"/>
       <c r="B41" s="23"/>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A42" s="36"/>
       <c r="B42" s="36"/>
       <c r="C42" s="36"/>

</xml_diff>

<commit_message>
"Updated SprintBurnDown and Finished LOG_IN Scenario from Salonika"
</commit_message>
<xml_diff>
--- a/Done/Sprint_Burndown_Chart_Template.xlsx
+++ b/Done/Sprint_Burndown_Chart_Template.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bbui1\Documents\GitHub\swe443\SWE443BankSystemBlue\Done\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Salonika/Desktop/GitRepo/SWE443BankSystemBlue/Done/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23040" windowHeight="9080"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown Chart Template" sheetId="5" r:id="rId1"/>
@@ -20,7 +20,15 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Burndown Chart Template'!$B$31:$V$40</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Burndown Chart Template'!$3:$5</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -30,7 +38,7 @@
     <author>Anne</author>
   </authors>
   <commentList>
-    <comment ref="E5" authorId="0" shapeId="0">
+    <comment ref="E5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -54,7 +62,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G6" authorId="0" shapeId="0">
+    <comment ref="G6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -78,7 +86,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H8" authorId="0" shapeId="0">
+    <comment ref="H8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -102,7 +110,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S8" authorId="0" shapeId="0">
+    <comment ref="S8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -116,7 +124,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J9" authorId="0" shapeId="0">
+    <comment ref="J9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -140,7 +148,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L9" authorId="0" shapeId="0">
+    <comment ref="L9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -165,7 +173,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S9" authorId="0" shapeId="0">
+    <comment ref="S9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -179,7 +187,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K10" authorId="0" shapeId="0">
+    <comment ref="K10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -193,7 +201,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O10" authorId="0" shapeId="0">
+    <comment ref="O10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -207,7 +215,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P10" authorId="0" shapeId="0">
+    <comment ref="P10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -319,7 +327,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -495,25 +503,25 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -522,20 +530,20 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -543,24 +551,24 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -569,7 +577,7 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -577,17 +585,17 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -597,7 +605,7 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -605,12 +613,12 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -619,27 +627,27 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -647,99 +655,99 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -747,78 +755,78 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -826,13 +834,13 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -841,60 +849,60 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1099,7 +1107,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1172,7 +1180,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -1185,43 +1193,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>18</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17</c:v>
+                  <c:v>22.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16</c:v>
+                  <c:v>21.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16</c:v>
+                  <c:v>21.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>21.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21</c:v>
+                  <c:v>26.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>19</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>14</c:v>
+                  <c:v>19.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>14</c:v>
+                  <c:v>19.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-89B2-4689-9D60-2A49D583E5FD}"/>
             </c:ext>
@@ -1260,43 +1268,43 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>18</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.2</c:v>
+                  <c:v>20.7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.399999999999999</c:v>
+                  <c:v>18.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.599999999999998</c:v>
+                  <c:v>16.1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10.799999999999997</c:v>
+                  <c:v>13.8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.9999999999999964</c:v>
+                  <c:v>11.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.1999999999999966</c:v>
+                  <c:v>9.199999999999995</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.3999999999999968</c:v>
+                  <c:v>6.899999999999996</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.599999999999997</c:v>
+                  <c:v>4.599999999999996</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.7999999999999969</c:v>
+                  <c:v>2.299999999999996</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-3.1086244689504383E-15</c:v>
+                  <c:v>-3.5527136788005E-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-89B2-4689-9D60-2A49D583E5FD}"/>
             </c:ext>
@@ -1311,11 +1319,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="414553768"/>
-        <c:axId val="414555728"/>
+        <c:axId val="956923856"/>
+        <c:axId val="956926944"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="414553768"/>
+        <c:axId val="956923856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1325,7 +1333,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="414555728"/>
+        <c:crossAx val="956926944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1333,7 +1341,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="414555728"/>
+        <c:axId val="956926944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1344,7 +1352,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="414553768"/>
+        <c:crossAx val="956923856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1424,7 +1432,7 @@
         <xdr:cNvPr id="9230" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E240000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000E240000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1493,9 +1501,9 @@
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -1523,31 +1531,14 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -1575,23 +1566,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1768,27 +1742,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="8" tint="0.79998168889431442"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:X42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="66.5546875" customWidth="1"/>
+    <col min="4" max="4" width="66.5" customWidth="1"/>
     <col min="5" max="15" width="10.6640625" customWidth="1"/>
     <col min="16" max="16" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10.6640625" customWidth="1"/>
-    <col min="24" max="24" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="25.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="49.8" x14ac:dyDescent="0.8">
+    <row r="1" spans="1:23" ht="50" x14ac:dyDescent="0.5">
       <c r="A1" s="36"/>
       <c r="B1" s="76" t="s">
         <v>24</v>
@@ -1815,7 +1789,7 @@
       <c r="V1" s="76"/>
       <c r="W1" s="76"/>
     </row>
-    <row r="2" spans="1:23" ht="33" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:23" ht="34" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="36"/>
       <c r="B2" s="77" t="s">
         <v>21</v>
@@ -1842,7 +1816,7 @@
       <c r="V2" s="77"/>
       <c r="W2" s="77"/>
     </row>
-    <row r="3" spans="1:23" s="2" customFormat="1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:23" s="2" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="34"/>
       <c r="B3" s="41"/>
       <c r="C3" s="42"/>
@@ -1867,7 +1841,7 @@
       <c r="V3" s="70"/>
       <c r="W3" s="44"/>
     </row>
-    <row r="4" spans="1:23" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A4" s="35"/>
       <c r="B4" s="37"/>
       <c r="C4" s="45" t="s">
@@ -1915,7 +1889,7 @@
       <c r="U4" s="38"/>
       <c r="W4" s="39"/>
     </row>
-    <row r="5" spans="1:23" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:23" s="3" customFormat="1" ht="31" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="35"/>
       <c r="B5" s="37"/>
       <c r="C5" s="25"/>
@@ -1963,7 +1937,7 @@
       <c r="U5" s="38"/>
       <c r="W5" s="39"/>
     </row>
-    <row r="6" spans="1:23" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:23" ht="34.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="36"/>
       <c r="B6" s="16"/>
       <c r="C6" s="26">
@@ -2004,7 +1978,7 @@
       <c r="V6" s="15"/>
       <c r="W6" s="17"/>
     </row>
-    <row r="7" spans="1:23" ht="18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:23" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" s="36"/>
       <c r="B7" s="16"/>
       <c r="C7" s="26">
@@ -2039,7 +2013,7 @@
       <c r="V7" s="17"/>
       <c r="W7" s="17"/>
     </row>
-    <row r="8" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="36"/>
       <c r="B8" s="16"/>
       <c r="C8" s="26">
@@ -2079,7 +2053,7 @@
       <c r="V8" s="17"/>
       <c r="W8" s="17"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" s="36"/>
       <c r="B9" s="16"/>
       <c r="C9" s="26">
@@ -2115,7 +2089,7 @@
       <c r="V9" s="17"/>
       <c r="W9" s="17"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" s="36"/>
       <c r="B10" s="16"/>
       <c r="C10" s="26">
@@ -2150,7 +2124,7 @@
       <c r="V10" s="17"/>
       <c r="W10" s="17"/>
     </row>
-    <row r="11" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="36"/>
       <c r="B11" s="16"/>
       <c r="C11" s="61">
@@ -2181,7 +2155,7 @@
       <c r="V11" s="20"/>
       <c r="W11" s="17"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" s="36"/>
       <c r="B12" s="68"/>
       <c r="C12" s="67">
@@ -2207,7 +2181,7 @@
       </c>
       <c r="W12" s="17"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" s="36"/>
       <c r="B13" s="68"/>
       <c r="C13" s="67">
@@ -2242,7 +2216,7 @@
       <c r="U13" s="13"/>
       <c r="W13" s="17"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" s="36"/>
       <c r="B14" s="68"/>
       <c r="C14" s="67">
@@ -2271,7 +2245,7 @@
       <c r="U14" s="13"/>
       <c r="W14" s="17"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" s="36"/>
       <c r="B15" s="68"/>
       <c r="C15" s="67">
@@ -2301,7 +2275,7 @@
       <c r="V15" s="58"/>
       <c r="W15" s="17"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" s="36"/>
       <c r="B16" s="68"/>
       <c r="C16" s="67">
@@ -2331,7 +2305,7 @@
       <c r="V16" s="58"/>
       <c r="W16" s="17"/>
     </row>
-    <row r="17" spans="1:24" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="36"/>
       <c r="B17" s="68"/>
       <c r="C17" s="67">
@@ -2363,7 +2337,7 @@
       <c r="V17" s="58"/>
       <c r="W17" s="17"/>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18" s="36"/>
       <c r="B18" s="68"/>
       <c r="C18" s="67">
@@ -2371,7 +2345,7 @@
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="5">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
@@ -2395,7 +2369,7 @@
       <c r="V18" s="58"/>
       <c r="W18" s="17"/>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
       <c r="B19" s="68"/>
       <c r="C19" s="67">
@@ -2425,7 +2399,7 @@
       <c r="V19" s="58"/>
       <c r="W19" s="17"/>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20" s="36"/>
       <c r="B20" s="68"/>
       <c r="C20" s="67">
@@ -2455,7 +2429,7 @@
       <c r="V20" s="58"/>
       <c r="W20" s="17"/>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21" s="36"/>
       <c r="B21" s="68"/>
       <c r="C21" s="67">
@@ -2485,7 +2459,7 @@
       <c r="V21" s="58"/>
       <c r="W21" s="17"/>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22" s="36"/>
       <c r="B22" s="68"/>
       <c r="C22" s="67">
@@ -2515,7 +2489,7 @@
       <c r="V22" s="58"/>
       <c r="W22" s="17"/>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A23" s="36"/>
       <c r="B23" s="68"/>
       <c r="C23" s="67">
@@ -2545,7 +2519,7 @@
       <c r="V23" s="58"/>
       <c r="W23" s="17"/>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24" s="36"/>
       <c r="B24" s="68"/>
       <c r="C24" s="67">
@@ -2575,7 +2549,7 @@
       <c r="V24" s="58"/>
       <c r="W24" s="17"/>
     </row>
-    <row r="25" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="36"/>
       <c r="B25" s="68"/>
       <c r="C25" s="67">
@@ -2605,7 +2579,7 @@
       <c r="V25" s="58"/>
       <c r="W25" s="17"/>
     </row>
-    <row r="26" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="36"/>
       <c r="B26" s="16"/>
       <c r="C26" s="48"/>
@@ -2614,47 +2588,47 @@
       </c>
       <c r="E26" s="65">
         <f>SUM(E6:E20)</f>
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F26" s="66">
         <f>E26-SUM(F6:F20)</f>
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G26" s="66">
         <f t="shared" ref="G26:O26" si="1">F26-SUM(G6:G20)</f>
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="H26" s="66">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="I26" s="66">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="J26" s="66">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="K26" s="66">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="L26" s="66">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="M26" s="66">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="N26" s="66">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="O26" s="66">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="P26" s="69"/>
       <c r="Q26" s="58"/>
@@ -2665,7 +2639,7 @@
       <c r="V26" s="58"/>
       <c r="W26" s="17"/>
     </row>
-    <row r="27" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="36"/>
       <c r="B27" s="16"/>
       <c r="C27" s="49"/>
@@ -2674,47 +2648,47 @@
       </c>
       <c r="E27" s="51">
         <f>E26</f>
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F27" s="52">
         <f t="shared" ref="F27:O27" si="2">E27-($E$26/10)</f>
-        <v>16.2</v>
+        <v>20.7</v>
       </c>
       <c r="G27" s="52">
         <f t="shared" si="2"/>
-        <v>14.399999999999999</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="H27" s="52">
         <f t="shared" si="2"/>
-        <v>12.599999999999998</v>
+        <v>16.099999999999998</v>
       </c>
       <c r="I27" s="52">
         <f t="shared" si="2"/>
-        <v>10.799999999999997</v>
+        <v>13.799999999999997</v>
       </c>
       <c r="J27" s="52">
         <f t="shared" si="2"/>
-        <v>8.9999999999999964</v>
+        <v>11.499999999999996</v>
       </c>
       <c r="K27" s="52">
         <f t="shared" si="2"/>
-        <v>7.1999999999999966</v>
+        <v>9.1999999999999957</v>
       </c>
       <c r="L27" s="52">
         <f t="shared" si="2"/>
-        <v>5.3999999999999968</v>
+        <v>6.8999999999999959</v>
       </c>
       <c r="M27" s="52">
         <f t="shared" si="2"/>
-        <v>3.599999999999997</v>
+        <v>4.5999999999999961</v>
       </c>
       <c r="N27" s="52">
         <f t="shared" si="2"/>
-        <v>1.7999999999999969</v>
+        <v>2.2999999999999963</v>
       </c>
       <c r="O27" s="53">
         <f t="shared" si="2"/>
-        <v>-3.1086244689504383E-15</v>
+        <v>-3.5527136788005009E-15</v>
       </c>
       <c r="P27" s="58"/>
       <c r="Q27" s="58"/>
@@ -2725,7 +2699,7 @@
       <c r="V27" s="58"/>
       <c r="W27" s="17"/>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A28" s="36"/>
       <c r="B28" s="16"/>
       <c r="C28" s="58"/>
@@ -2750,7 +2724,7 @@
       <c r="V28" s="58"/>
       <c r="W28" s="17"/>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A29" s="36"/>
       <c r="B29" s="16"/>
       <c r="C29" s="58"/>
@@ -2775,7 +2749,7 @@
       <c r="V29" s="58"/>
       <c r="W29" s="17"/>
     </row>
-    <row r="30" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="36"/>
       <c r="B30" s="18"/>
       <c r="C30" s="19"/>
@@ -2800,23 +2774,23 @@
       <c r="V30" s="54"/>
       <c r="W30" s="20"/>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A31" s="36"/>
       <c r="X31" s="23"/>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A32" s="36"/>
       <c r="X32" s="23"/>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A33" s="36"/>
       <c r="X33" s="23"/>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A34" s="36"/>
       <c r="X34" s="23"/>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A35" s="36"/>
       <c r="B35" s="13"/>
       <c r="C35" s="58"/>
@@ -2842,7 +2816,7 @@
       <c r="W35" s="13"/>
       <c r="X35" s="23"/>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A36" s="36"/>
       <c r="B36" s="13"/>
       <c r="C36" s="58"/>
@@ -2868,7 +2842,7 @@
       <c r="W36" s="13"/>
       <c r="X36" s="23"/>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A37" s="36"/>
       <c r="B37" s="13"/>
       <c r="C37" s="58"/>
@@ -2894,7 +2868,7 @@
       <c r="W37" s="13"/>
       <c r="X37" s="23"/>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A38" s="36"/>
       <c r="B38" s="13"/>
       <c r="C38" s="58"/>
@@ -2920,7 +2894,7 @@
       <c r="W38" s="13"/>
       <c r="X38" s="23"/>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A39" s="36"/>
       <c r="B39" s="13"/>
       <c r="C39" s="58"/>
@@ -2946,7 +2920,7 @@
       <c r="W39" s="13"/>
       <c r="X39" s="23"/>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A40" s="36"/>
       <c r="B40" s="13"/>
       <c r="C40" s="13"/>
@@ -2971,11 +2945,11 @@
       <c r="W40" s="13"/>
       <c r="X40" s="23"/>
     </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A41" s="36"/>
       <c r="B41" s="23"/>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A42" s="36"/>
       <c r="B42" s="36"/>
       <c r="C42" s="36"/>

</xml_diff>